<commit_message>
first complete site spreadsheet to track overlay
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-microsoft-iis-8.5-site-stig-overlay_20181224.xlsx
+++ b/cms-ars-3.1-high-microsoft-iis-8.5-site-stig-overlay_20181224.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BF39779F-9E33-43E3-9423-D0FEC027C6F6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{072B95A2-1F87-494F-9DC8-8E0E122B9DBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="IIS8.5Site" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IIS8.5Site'!$A$1:$X$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IIS8.5Site'!$A$1:$X$55</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="470">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -3189,6 +3189,12 @@
 Without sufficient information establishing when the log event occurred, investigation into the cause of event is severely hindered. Log record content that may be necessary to satisfy the requirement of this control includes, but is not limited to, time stamps, source and destination IP addresses, user/process identifiers, event descriptions, application-specific events, success/fail indications, file names involved, access control, or flow control rules invoked.
 Satisfies: SRG-APP-000092-WSR-000055, SRG-APP-000093-WSR-000053</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">describe "For this CMS ARS 3.1 overlay, this control must be reviewed manually" do 
+skip "For this CMS ARS 3.1 overlay, this control must be reviewed manually"
+end
+</t>
   </si>
 </sst>
 </file>
@@ -4115,11 +4121,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X33" sqref="X33"/>
+      <selection pane="bottomRight" activeCell="AE38" sqref="AE38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -6349,7 +6355,9 @@
       <c r="X38" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="Y38" s="2"/>
+      <c r="Y38" s="6" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="39" spans="1:25" ht="409.6">
       <c r="A39" s="5" t="s">
@@ -7323,7 +7331,7 @@
       <c r="Y55" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:X55" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updates relative to 12/17 version
removed comments/editing questions from first column
added NOTES column, removed CMS NIST column
updated:
V-76783
V-76789
V-76791
V-76809
V-76817, 19, 21, 23, 25, 27
V-76839, 41
V-76847, 49
and remaining rows
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-microsoft-iis-8.5-site-stig-overlay_20181224.xlsx
+++ b/cms-ars-3.1-high-microsoft-iis-8.5-site-stig-overlay_20181224.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{072B95A2-1F87-494F-9DC8-8E0E122B9DBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{023AE278-5192-4653-81EC-DD668E021A9E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2137,14 +2137,6 @@
     <t>IISW-SI-000264</t>
   </si>
   <si>
-    <t>V-76789
-What are the custom fields and can we support this</t>
-  </si>
-  <si>
-    <t>V-76791
-same as above</t>
-  </si>
-  <si>
     <r>
       <t>Follow the procedures below for each site hosted on the IIS 8.5 web server:
 Open the IIS 8.5 Manager.
@@ -3195,6 +3187,13 @@
 skip "For this CMS ARS 3.1 overlay, this control must be reviewed manually"
 end
 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V-76789
+</t>
+  </si>
+  <si>
+    <t>V-76791</t>
   </si>
 </sst>
 </file>
@@ -4121,11 +4120,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE38" sqref="AE38"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -4229,7 +4228,7 @@
         <v>23</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="273.60000000000002">
@@ -4256,10 +4255,10 @@
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="8" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -4519,7 +4518,7 @@
     </row>
     <row r="7" spans="1:25" ht="409.6">
       <c r="A7" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>25</v>
@@ -4537,7 +4536,7 @@
         <v>68</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
@@ -4573,7 +4572,7 @@
         <v>103</v>
       </c>
       <c r="Y7" s="7" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="409.6">
@@ -4692,7 +4691,7 @@
     </row>
     <row r="10" spans="1:25" ht="409.6">
       <c r="A10" s="5" t="s">
-        <v>439</v>
+        <v>468</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>25</v>
@@ -4749,7 +4748,7 @@
     </row>
     <row r="11" spans="1:25" ht="409.6">
       <c r="A11" s="5" t="s">
-        <v>440</v>
+        <v>469</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>25</v>
@@ -5170,7 +5169,7 @@
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="4" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>160</v>
@@ -5202,7 +5201,7 @@
         <v>161</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="403.2">
@@ -5225,7 +5224,7 @@
         <v>166</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
@@ -5489,7 +5488,7 @@
         <v>249</v>
       </c>
       <c r="Y23" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="244.8">
@@ -5548,7 +5547,7 @@
         <v>249</v>
       </c>
       <c r="Y24" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="216">
@@ -5607,7 +5606,7 @@
         <v>249</v>
       </c>
       <c r="Y25" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="216">
@@ -5666,7 +5665,7 @@
         <v>249</v>
       </c>
       <c r="Y26" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="216">
@@ -5725,7 +5724,7 @@
         <v>249</v>
       </c>
       <c r="Y27" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="259.2">
@@ -5784,7 +5783,7 @@
         <v>249</v>
       </c>
       <c r="Y28" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="216">
@@ -6245,7 +6244,7 @@
     </row>
     <row r="37" spans="1:25" ht="409.6">
       <c r="A37" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>25</v>
@@ -6260,14 +6259,14 @@
         <v>312</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>313</v>
@@ -6317,17 +6316,17 @@
         <v>318</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -6356,7 +6355,7 @@
         <v>319</v>
       </c>
       <c r="Y38" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="39" spans="1:25" ht="409.6">
@@ -6535,7 +6534,7 @@
         <v>346</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>347</v>
@@ -6586,7 +6585,7 @@
         <v>354</v>
       </c>
       <c r="Y42" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="43" spans="1:25" ht="216">
@@ -6670,7 +6669,7 @@
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="4" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J44" s="2" t="s">
         <v>369</v>
@@ -6727,7 +6726,7 @@
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>374</v>
@@ -6784,7 +6783,7 @@
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>379</v>
@@ -6841,7 +6840,7 @@
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J47" s="2" t="s">
         <v>385</v>
@@ -7290,17 +7289,17 @@
         <v>438</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>

</xml_diff>

<commit_message>
updating spreadsheet to have correct banner text.
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-high-microsoft-iis-8.5-site-stig-overlay_20181224.xlsx
+++ b/cms-ars-3.1-high-microsoft-iis-8.5-site-stig-overlay_20181224.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars3.1-high-microsoft-iis-8.5-site-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{023AE278-5192-4653-81EC-DD668E021A9E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352AA815-DE9F-6C45-9EA6-C92C27AB73CE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="19220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IIS8.5Site" sheetId="1" r:id="rId1"/>
@@ -2966,56 +2966,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Note: This requirement is only applicable for private </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CMS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> websites.
-If a banner is required, the following banner page must be in place: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* This warning banner provides privacy and security notices consistent with applicable federal laws, directives, and other federal guidance for accessing this Government system, which includes (1) this computer network, (2) all computers connected to this network, and (3) all devices and storage media attached to this network or to a computer on this network.  * This system is provided for Government authorized use only.  * Unauthorized or improper use of this system is prohibited and may result in disciplinary action and/or civil and criminal penalties.  * Personal use of social media and networking sites on this system is limited as to not interfere with official work duties and is subject to monitoring.  * By using this system, you understand and consent to the following:     - The Government may monitor, record, and audit your system usage, including usage of personal devices and email systems for official duties or to conduct HHS business. Therefore, you have no reasonable expectation of privacy regarding any communication or data transiting or stored on this system. At any time, and for any lawful Government purpose, the government may monitor, intercept, and search and seize any communication or data transiting or stored on this system.     - Any communication or data transiting or stored on this system may be disclosed or used for any lawful Government purposeb. Retains the notification message or banner on the screen until users take explicit actions to log on to or further access the information system; and c. For publicly accessible systems:   1. Displays system use information when appropriate, before granting further access;   2. Displays references, if any, to monitoring, recording, or auditing that are consistent with privacy accommodations for such systems that generally prohibit those activities; and   3. Includes a description of the authorized uses of the system.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-If the access-controlled website does not display this banner page before entry, this is a finding.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Access the IIS 8.5 IIS Manager.
 Click the IIS 8.5 server.
 Select "Configuration Editor" under the "Management" section.
@@ -3194,6 +3144,56 @@
   </si>
   <si>
     <t>V-76791</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Note: This requirement is only applicable for private </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CMS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> websites.
+If a banner is required, the following banner page must be in place: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* This warning banner provides privacy and security notices consistent with applicable federal laws, directives, and other federal guidance for accessing this Government system, which includes (1) this computer network, (2) all computers connected to this network, and (3) all devices and storage media attached to this network or to a computer on this network.  * This system is provided for Government authorized use only.  * Unauthorized or improper use of this system is prohibited and may result in disciplinary action and/or civil and criminal penalties.  * Personal use of social media and networking sites on this system is limited as to not interfere with official work duties and is subject to monitoring.  * By using this system, you understand and consent to the following:     - The Government may monitor, record, and audit your system usage, including usage of personal devices and email systems for official duties or to conduct HHS business. Therefore, you have no reasonable expectation of privacy regarding any communication or data transiting or stored on this system. At any time, and for any lawful Government purpose, the government may monitor, intercept, and search and seize any communication or data transiting or stored on this system.     - Any communication or data transiting or stored on this system may be disclosed or used for any lawful Government purpose.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+If the access-controlled website does not display this banner page before entry, this is a finding.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4120,41 +4120,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="213" zoomScaleNormal="213" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="J55" sqref="J55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="1" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="25" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.77734375" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="41.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="41.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="40.6640625" style="1" customWidth="1"/>
-    <col min="11" max="12" width="8.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="8.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="1" hidden="1" customWidth="1"/>
     <col min="14" max="15" width="8.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="5.44140625" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="8.44140625" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="8.109375" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="8.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="8.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5" style="1" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="8.33203125" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="8.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5" style="1" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="8.6640625" style="1" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="7.109375" style="1" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="7.1640625" style="1" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.109375" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.77734375" style="1"/>
+    <col min="25" max="25" width="15.1640625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="17.55" customHeight="1">
+    <row r="1" spans="1:25" ht="17.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="273.60000000000002">
+    <row r="2" spans="1:25" ht="304">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -4255,10 +4255,10 @@
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>464</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>465</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -4402,7 +4402,7 @@
       </c>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="1:25" ht="302.39999999999998">
+    <row r="5" spans="1:25" ht="304">
       <c r="A5" s="5" t="s">
         <v>50</v>
       </c>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="Y5" s="2"/>
     </row>
-    <row r="6" spans="1:25" ht="302.39999999999998">
+    <row r="6" spans="1:25" ht="304">
       <c r="A6" s="5" t="s">
         <v>59</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>68</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
@@ -4632,7 +4632,7 @@
       </c>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:25" ht="409.05" customHeight="1">
+    <row r="9" spans="1:25" ht="409" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>79</v>
       </c>
@@ -4691,7 +4691,7 @@
     </row>
     <row r="10" spans="1:25" ht="409.6">
       <c r="A10" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>25</v>
@@ -4748,7 +4748,7 @@
     </row>
     <row r="11" spans="1:25" ht="409.6">
       <c r="A11" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>25</v>
@@ -4803,7 +4803,7 @@
       </c>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25" ht="360">
+    <row r="12" spans="1:25" ht="380">
       <c r="A12" s="5" t="s">
         <v>104</v>
       </c>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" ht="288">
+    <row r="14" spans="1:25" ht="304">
       <c r="A14" s="5" t="s">
         <v>122</v>
       </c>
@@ -4974,7 +4974,7 @@
       </c>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" ht="288">
+    <row r="15" spans="1:25" ht="304">
       <c r="A15" s="5" t="s">
         <v>130</v>
       </c>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="331.2">
+    <row r="18" spans="1:25" ht="335">
       <c r="A18" s="3" t="s">
         <v>154</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="403.2">
+    <row r="19" spans="1:25" ht="409.6">
       <c r="A19" s="3" t="s">
         <v>162</v>
       </c>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" ht="230.4">
+    <row r="22" spans="1:25" ht="240">
       <c r="A22" s="5" t="s">
         <v>189</v>
       </c>
@@ -5432,7 +5432,7 @@
       </c>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" ht="216">
+    <row r="23" spans="1:25" ht="224">
       <c r="A23" s="3" t="s">
         <v>198</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="244.8">
+    <row r="24" spans="1:25" ht="272">
       <c r="A24" s="3" t="s">
         <v>206</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="216">
+    <row r="25" spans="1:25" ht="224">
       <c r="A25" s="3" t="s">
         <v>213</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="216">
+    <row r="26" spans="1:25" ht="224">
       <c r="A26" s="3" t="s">
         <v>220</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="216">
+    <row r="27" spans="1:25" ht="224">
       <c r="A27" s="3" t="s">
         <v>227</v>
       </c>
@@ -5727,7 +5727,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="259.2">
+    <row r="28" spans="1:25" ht="256">
       <c r="A28" s="3" t="s">
         <v>234</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="216">
+    <row r="29" spans="1:25" ht="240">
       <c r="A29" s="5" t="s">
         <v>241</v>
       </c>
@@ -5843,7 +5843,7 @@
       </c>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" ht="403.2">
+    <row r="30" spans="1:25" ht="409.6">
       <c r="A30" s="5" t="s">
         <v>250</v>
       </c>
@@ -5900,7 +5900,7 @@
       </c>
       <c r="Y30" s="2"/>
     </row>
-    <row r="31" spans="1:25" ht="216">
+    <row r="31" spans="1:25" ht="240">
       <c r="A31" s="5" t="s">
         <v>259</v>
       </c>
@@ -5957,7 +5957,7 @@
       </c>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" ht="244.8">
+    <row r="32" spans="1:25" ht="272">
       <c r="A32" s="5" t="s">
         <v>267</v>
       </c>
@@ -6014,7 +6014,7 @@
       </c>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:25" ht="288">
+    <row r="33" spans="1:25" ht="304">
       <c r="A33" s="5" t="s">
         <v>275</v>
       </c>
@@ -6071,7 +6071,7 @@
       </c>
       <c r="Y33" s="2"/>
     </row>
-    <row r="34" spans="1:25" ht="374.4">
+    <row r="34" spans="1:25" ht="409.6">
       <c r="A34" s="5" t="s">
         <v>284</v>
       </c>
@@ -6299,7 +6299,7 @@
       </c>
       <c r="Y37" s="2"/>
     </row>
-    <row r="38" spans="1:25" ht="388.8">
+    <row r="38" spans="1:25" ht="409.6">
       <c r="A38" s="3" t="s">
         <v>315</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>319</v>
       </c>
       <c r="Y38" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="39" spans="1:25" ht="409.6">
@@ -6415,7 +6415,7 @@
       </c>
       <c r="Y39" s="2"/>
     </row>
-    <row r="40" spans="1:25" ht="288">
+    <row r="40" spans="1:25" ht="304">
       <c r="A40" s="5" t="s">
         <v>329</v>
       </c>
@@ -6588,7 +6588,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="216">
+    <row r="43" spans="1:25" ht="208">
       <c r="A43" s="5" t="s">
         <v>355</v>
       </c>
@@ -6645,7 +6645,7 @@
       </c>
       <c r="Y43" s="2"/>
     </row>
-    <row r="44" spans="1:25" ht="316.8">
+    <row r="44" spans="1:25" ht="335">
       <c r="A44" s="3" t="s">
         <v>364</v>
       </c>
@@ -6702,7 +6702,7 @@
       </c>
       <c r="Y44" s="2"/>
     </row>
-    <row r="45" spans="1:25" ht="403.2">
+    <row r="45" spans="1:25" ht="409.6">
       <c r="A45" s="3" t="s">
         <v>370</v>
       </c>
@@ -6759,7 +6759,7 @@
       </c>
       <c r="Y45" s="2"/>
     </row>
-    <row r="46" spans="1:25" ht="316.8">
+    <row r="46" spans="1:25" ht="335">
       <c r="A46" s="3" t="s">
         <v>375</v>
       </c>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="Y46" s="2"/>
     </row>
-    <row r="47" spans="1:25" ht="374.4">
+    <row r="47" spans="1:25" ht="365">
       <c r="A47" s="3" t="s">
         <v>380</v>
       </c>
@@ -6873,7 +6873,7 @@
       </c>
       <c r="Y47" s="2"/>
     </row>
-    <row r="48" spans="1:25" ht="216">
+    <row r="48" spans="1:25" ht="224">
       <c r="A48" s="5" t="s">
         <v>386</v>
       </c>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="Y48" s="2"/>
     </row>
-    <row r="49" spans="1:25" ht="316.8">
+    <row r="49" spans="1:25" ht="350">
       <c r="A49" s="5" t="s">
         <v>393</v>
       </c>
@@ -6987,7 +6987,7 @@
       </c>
       <c r="Y49" s="2"/>
     </row>
-    <row r="50" spans="1:25" ht="230.4">
+    <row r="50" spans="1:25" ht="224">
       <c r="A50" s="5" t="s">
         <v>400</v>
       </c>
@@ -7044,7 +7044,7 @@
       </c>
       <c r="Y50" s="2"/>
     </row>
-    <row r="51" spans="1:25" ht="273.60000000000002">
+    <row r="51" spans="1:25" ht="304">
       <c r="A51" s="5" t="s">
         <v>407</v>
       </c>
@@ -7101,7 +7101,7 @@
       </c>
       <c r="Y51" s="2"/>
     </row>
-    <row r="52" spans="1:25" ht="360">
+    <row r="52" spans="1:25" ht="365">
       <c r="A52" s="5" t="s">
         <v>414</v>
       </c>
@@ -7215,7 +7215,7 @@
       </c>
       <c r="Y53" s="2"/>
     </row>
-    <row r="54" spans="1:25" ht="288">
+    <row r="54" spans="1:25" ht="320">
       <c r="A54" s="5" t="s">
         <v>429</v>
       </c>
@@ -7296,7 +7296,7 @@
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>462</v>

</xml_diff>